<commit_message>
Site updated: 2018-07-25 15:09:31
</commit_message>
<xml_diff>
--- a/2018/04/20/companylist/company.xlsx
+++ b/2018/04/20/companylist/company.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="24420" windowHeight="14520"/>
+    <workbookView xWindow="780" yWindow="940" windowWidth="24420" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Tier 1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Tier 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
   <si>
     <t>company</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -284,12 +285,55 @@
     <t>fitech</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Morganstanley</t>
+  </si>
+  <si>
+    <t>http://www.1point3acres.com/bbs/thread-429994-1-1.html</t>
+  </si>
+  <si>
+    <t>morganrefer@gmail.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://careers.tableau.com/listing</t>
+  </si>
+  <si>
+    <t>tableaureferrals@gmail.com</t>
+  </si>
+  <si>
+    <t>https://goo.gl/9wzEu9</t>
+  </si>
+  <si>
+    <t>Tableau</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://careers.microsoft.com/us/en</t>
+  </si>
+  <si>
+    <t>2018mshire@gmail.com</t>
+  </si>
+  <si>
+    <t>refer.microsoft.2018@gmail.com</t>
+  </si>
+  <si>
+    <t>https://goo.gl/f6xqb3</t>
+  </si>
+  <si>
+    <t>appleissrefer@gmail.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -304,6 +348,12 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFBBBBBB"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -323,6 +373,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color rgb="FF555555"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -330,6 +387,20 @@
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF555555"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -395,30 +466,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -739,7 +822,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -777,7 +860,7 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
@@ -785,10 +868,10 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -796,7 +879,7 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
@@ -807,18 +890,18 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -826,31 +909,45 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:7" ht="21">
+      <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17">
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D14" t="s">
@@ -858,35 +955,41 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:7">
       <c r="B17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="2:4">
+      <c r="D17" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
       <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:7">
       <c r="B21" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D21" t="s">
         <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -907,6 +1010,7 @@
     <hyperlink ref="C15" r:id="rId13"/>
     <hyperlink ref="C21" r:id="rId14"/>
     <hyperlink ref="C19" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -917,7 +1021,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -952,10 +1056,10 @@
       <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -963,7 +1067,7 @@
       <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -971,7 +1075,7 @@
       <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D6" t="s">
@@ -1003,14 +1107,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:7">
       <c r="B18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:7">
       <c r="B20" t="s">
         <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1027,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1072,28 +1179,56 @@
       <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>55</v>
       </c>
       <c r="G4" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16">
+      <c r="B6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1102,6 +1237,9 @@
     <hyperlink ref="D2" r:id="rId1" display="mailto:jpmc.referral815@gmail.com"/>
     <hyperlink ref="E2" r:id="rId2" display="https://jobs.jpmorganchase.com/"/>
     <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="E8" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6" display="mailto:tableaureferrals@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Site updated: 2018-07-30 14:14:27
</commit_message>
<xml_diff>
--- a/2018/04/20/companylist/company.xlsx
+++ b/2018/04/20/companylist/company.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="24420" windowHeight="14520"/>
+    <workbookView xWindow="780" yWindow="940" windowWidth="24420" windowHeight="14520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tier 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t>company</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -328,12 +328,48 @@
     <t>appleissrefer@gmail.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>https://goo.gl/rdNMgN</t>
+  </si>
+  <si>
+    <t>reffer3831@gmail.com</t>
+  </si>
+  <si>
+    <t>https://goo.gl/zoVi8a</t>
+  </si>
+  <si>
+    <t>gsuperreferal@google.com</t>
+  </si>
+  <si>
+    <t>https://goo.gl/LhXA5k</t>
+  </si>
+  <si>
+    <t>gnotnil@yahoo.com</t>
+  </si>
+  <si>
+    <t>shachikunewgrad@gmail.com</t>
+  </si>
+  <si>
+    <t>Circle/Poloniex</t>
+  </si>
+  <si>
+    <t>https://goo.gl/r5QXcy</t>
+  </si>
+  <si>
+    <t>Forescout</t>
+  </si>
+  <si>
+    <t>liusiyu0323@gmail.com</t>
+  </si>
+  <si>
+    <t>https://goo.gl/4dyiDz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -443,6 +479,28 @@
       <family val="1"/>
       <charset val="136"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF555555"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF555555"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -470,7 +528,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -502,6 +560,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -819,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -875,6 +942,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:7">
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>2</v>
@@ -978,6 +1053,14 @@
         <v>36</v>
       </c>
     </row>
+    <row r="20" spans="2:7">
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="21" spans="2:7">
       <c r="B21" t="s">
         <v>33</v>
@@ -990,6 +1073,14 @@
       </c>
       <c r="G21" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="17">
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1011,6 +1102,7 @@
     <hyperlink ref="C21" r:id="rId14"/>
     <hyperlink ref="C19" r:id="rId15"/>
     <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D20" r:id="rId17" display="mailto:gnotnil@yahoo.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1021,7 +1113,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1134,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1231,6 +1323,28 @@
         <v>65</v>
       </c>
     </row>
+    <row r="9" spans="1:7" ht="18">
+      <c r="B9" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="23">
+      <c r="B10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1240,6 +1354,7 @@
     <hyperlink ref="D6" r:id="rId4"/>
     <hyperlink ref="E8" r:id="rId5"/>
     <hyperlink ref="D8" r:id="rId6" display="mailto:tableaureferrals@gmail.com"/>
+    <hyperlink ref="D10" r:id="rId7" display="mailto:liusiyu0323@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Site updated: 2018-07-30 14:43:56
</commit_message>
<xml_diff>
--- a/2018/04/20/companylist/company.xlsx
+++ b/2018/04/20/companylist/company.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="24420" windowHeight="14520" activeTab="2"/>
+    <workbookView xWindow="780" yWindow="940" windowWidth="24420" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Tier 1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Tier 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -888,7 +887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1228,7 +1227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Site updated: 2018-08-08 17:14:07
</commit_message>
<xml_diff>
--- a/2018/04/20/companylist/company.xlsx
+++ b/2018/04/20/companylist/company.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="24420" windowHeight="14520"/>
+    <workbookView xWindow="780" yWindow="940" windowWidth="24420" windowHeight="14520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tier 1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Tier 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -887,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1111,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Site updated: 2018-08-21 16:54:40
</commit_message>
<xml_diff>
--- a/2018/04/20/companylist/company.xlsx
+++ b/2018/04/20/companylist/company.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="24420" windowHeight="14520" activeTab="1"/>
+    <workbookView xWindow="760" yWindow="920" windowWidth="24420" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Tier 1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Tier 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
   <si>
     <t>company</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,29 +44,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://goo.gl/MkCvdg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fancyusc@gmail.com</t>
-  </si>
-  <si>
-    <t>6/21 end</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>facebooksde@gmail.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://goo.gl/N9CjJA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">fbreferral.anyposition@gmail.com </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tier</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -91,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://www.1point3acres.com/bbs/thread-429788-1-1.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Linkedin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,20 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">https://goo.gl/8jBf3T, </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>infinity.730@outlook.com</t>
-  </si>
-  <si>
-    <t>https://goo.gl/Kga1fu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>referalamazon65@gmail.com</t>
-  </si>
-  <si>
     <t>Paypal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -160,17 +118,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">https://goo.gl/vw1cQW </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>diuhezi@gmail.com</t>
-  </si>
-  <si>
-    <t>https://goo.gl/jD8siQ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Adobe</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -181,13 +128,6 @@
   <si>
     <t>Airbnb</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">https://goo.gl/z8k4st </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>referralairbnb@gmail.com</t>
   </si>
   <si>
     <t>Uber</t>
@@ -329,24 +269,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://goo.gl/rdNMgN</t>
-  </si>
-  <si>
-    <t>reffer3831@gmail.com</t>
-  </si>
-  <si>
     <t>https://goo.gl/zoVi8a</t>
   </si>
   <si>
     <t>gsuperreferal@google.com</t>
   </si>
   <si>
-    <t>https://goo.gl/LhXA5k</t>
-  </si>
-  <si>
-    <t>gnotnil@yahoo.com</t>
-  </si>
-  <si>
     <t>shachikunewgrad@gmail.com</t>
   </si>
   <si>
@@ -363,12 +291,62 @@
   </si>
   <si>
     <t>https://goo.gl/4dyiDz</t>
+  </si>
+  <si>
+    <t>Walmart Sam's Club Technology</t>
+  </si>
+  <si>
+    <t>8/14, 8/29 tech interview</t>
+  </si>
+  <si>
+    <t>http://www.1point3acres.com/bbs/thread-437804-1-1.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/15, 8/17 recruiter </t>
+  </si>
+  <si>
+    <t>http://www.1point3acres.com/bbs/thread-435755-1-1.html</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/careers/jobs/a0I1H00000LCQMWUA5/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/careers/jobs/a0I1H00000LBiNYUA1/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/careers/jobs/a0I1200000JA4R2EAL/</t>
+  </si>
+  <si>
+    <t>8/16, 8/17 confirm letter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kevin lai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.jobs/zh/jobs/697789/2019-software-development-engineer-united-states</t>
+  </si>
+  <si>
+    <t>https://goo.gl/koXpJ8</t>
+  </si>
+  <si>
+    <t>https://goo.gl/Xguhhv</t>
+  </si>
+  <si>
+    <t>https://goo.gl/h4dK78</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/jobs/listing/1234094</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+  </numFmts>
   <fonts count="17">
     <font>
       <sz val="12"/>
@@ -528,7 +506,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -569,6 +547,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -888,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -899,25 +883,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -925,184 +909,162 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="C4" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16">
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16">
+      <c r="C6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="16">
+      <c r="C7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="16">
+      <c r="C8" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="21">
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17">
       <c r="C13" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="C15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
+        <v>75</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16">
+      <c r="C15" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="16">
       <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="14">
+        <v>43331</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="C20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:7" ht="16">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" t="s">
-        <v>61</v>
+      <c r="G21" s="14">
+        <v>43333</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="17">
-      <c r="C22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="C22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1"/>
-    <hyperlink ref="D6" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
-    <hyperlink ref="D7" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
-    <hyperlink ref="C3" r:id="rId6"/>
-    <hyperlink ref="D3" r:id="rId7"/>
-    <hyperlink ref="C7" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C9" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C14" r:id="rId12"/>
-    <hyperlink ref="C15" r:id="rId13"/>
-    <hyperlink ref="C21" r:id="rId14"/>
-    <hyperlink ref="C19" r:id="rId15"/>
-    <hyperlink ref="D17" r:id="rId16"/>
-    <hyperlink ref="D20" r:id="rId17" display="mailto:gnotnil@yahoo.com"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="C10" r:id="rId4"/>
+    <hyperlink ref="C9" r:id="rId5"/>
+    <hyperlink ref="C12" r:id="rId6"/>
+    <hyperlink ref="D17" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1110,35 +1072,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1146,70 +1108,81 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16">
       <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="15">
+        <v>43331</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="16">
+      <c r="B22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1191,6 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1240,25 +1212,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1266,44 +1238,44 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" s="8" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16">
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16">
@@ -1311,38 +1283,38 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18">
       <c r="B9" s="13" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="23">
       <c r="B10" s="12" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>